<commit_message>
Added tab switching for GHG molecule charts
</commit_message>
<xml_diff>
--- a/3-climate-change/data/ghg_mole_fraction.xlsx
+++ b/3-climate-change/data/ghg_mole_fraction.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CO2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>year</t>
   </si>
@@ -34,6 +35,12 @@
   </si>
   <si>
     <t xml:space="preserve"> n2o global mean(ppb)</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>PPM</t>
   </si>
 </sst>
 </file>
@@ -436,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -930,6 +937,275 @@
       </c>
       <c r="D35">
         <v>1824</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B2">
+        <v>344.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1985</v>
+      </c>
+      <c r="B3">
+        <v>345.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B4">
+        <v>347.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>1987</v>
+      </c>
+      <c r="B5">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B6">
+        <v>351.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B7">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B8">
+        <v>354.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B9">
+        <v>355.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B10">
+        <v>356.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B11">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B12">
+        <v>358.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B13">
+        <v>360.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B14">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B15">
+        <v>363.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B16">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B17">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B18">
+        <v>369.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B19">
+        <v>370.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B20">
+        <v>372.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B21">
+        <v>375.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B22">
+        <v>377.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B23">
+        <v>379.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B24">
+        <v>381.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B25">
+        <v>383.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B26">
+        <v>385.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B27">
+        <v>386.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B28">
+        <v>388.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B29">
+        <v>390.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B30">
+        <v>393.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B31">
+        <v>396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>